<commit_message>
started working on third module
</commit_message>
<xml_diff>
--- a/_zakres_modulu_analizy_rynkowe.xlsx
+++ b/_zakres_modulu_analizy_rynkowe.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Majesty/Documents/Docs/Firma/Auxilium/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawidpylak/Documents/Economic_Indicators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71BB385C-3382-ED48-A183-DA704C22CA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79B25E3-651C-9741-9616-C1A53156F78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1500" windowWidth="24480" windowHeight="13620" xr2:uid="{733F56BF-16FE-8A4F-A19A-9398D47A6F3B}"/>
+    <workbookView xWindow="-33600" yWindow="11300" windowWidth="33600" windowHeight="20500" xr2:uid="{733F56BF-16FE-8A4F-A19A-9398D47A6F3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -496,32 +496,65 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -529,43 +562,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Procentowy" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -606,9 +606,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -646,7 +646,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -752,7 +752,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -904,14 +904,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3F200E-8475-2241-A980-08C03FE6C607}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.25" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4.25" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" style="14" customWidth="1"/>
-    <col min="4" max="7" width="25" style="9" customWidth="1"/>
+    <col min="3" max="3" width="25" style="13" customWidth="1"/>
+    <col min="4" max="7" width="25" style="8" customWidth="1"/>
     <col min="8" max="16384" width="13.25" style="7"/>
   </cols>
   <sheetData>
@@ -938,23 +940,23 @@
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="14">
         <v>40461</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="340.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
@@ -969,68 +971,68 @@
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C7" s="20">
+      <c r="C7" s="16">
         <v>1012</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="13">
+      <c r="E7" s="24"/>
+      <c r="F7" s="12">
         <v>1</v>
       </c>
-      <c r="G7" s="13"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C8" s="20">
+      <c r="C8" s="16">
         <v>1315</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C9" s="20"/>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C10" s="20"/>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="F11" s="23">
+      <c r="F11" s="17">
         <f>SUM(F7:F10)</f>
         <v>1</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="17">
         <f>SUM(G7:G10)</f>
         <v>0</v>
       </c>
@@ -1048,117 +1050,117 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26" t="s">
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="C15" s="24"/>
-      <c r="D15" s="10" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="26"/>
+      <c r="G15" s="27"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="2:7" ht="39" x14ac:dyDescent="0.15">
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>1000</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>2000</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>2500</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C18" s="20"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="11"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C19" s="20"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="11"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="2:7" ht="39" x14ac:dyDescent="0.15">
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="11">
         <v>1000</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="11">
         <v>2000</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="11">
         <v>2500</v>
       </c>
-      <c r="G21" s="11"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C22" s="20"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="11"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C23" s="20"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="11"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="2:7" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="4" t="s">
@@ -1173,104 +1175,114 @@
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="2:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="19" t="s">
+      <c r="E25" s="22"/>
+      <c r="F25" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="24"/>
-      <c r="D26" s="15" t="s">
+      <c r="C26" s="20"/>
+      <c r="D26" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="13">
+      <c r="E26" s="18"/>
+      <c r="F26" s="12">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="24"/>
-      <c r="D27" s="15" t="s">
+      <c r="C27" s="20"/>
+      <c r="D27" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="13">
+      <c r="E27" s="18"/>
+      <c r="F27" s="12">
         <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="24"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="13"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" spans="2:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C29" s="24"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="13"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C30" s="24"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="23">
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="17">
         <f>SUM(F26:F29)</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="264.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
     </row>
     <row r="32" spans="2:7" ht="264.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="3:7" ht="264.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="3:7" ht="264.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="D31:G31"/>
     <mergeCell ref="D32:G32"/>
     <mergeCell ref="D33:G33"/>
@@ -1284,16 +1296,6 @@
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <conditionalFormatting sqref="F11:G11">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">

</xml_diff>